<commit_message>
add information about IDB ports
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\prj_ASU\AMKP\S7Proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\prj_ASU\AMKP\git\gasCollectionPrj\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="279">
   <si>
     <t>Устройство</t>
   </si>
@@ -1413,6 +1413,37 @@
   </si>
   <si>
     <t>порт 39</t>
+  </si>
+  <si>
+    <t>2000/2001</t>
+  </si>
+  <si>
+    <t>Порт IDB 
+(cur/sum data)</t>
+  </si>
+  <si>
+    <t>2002/2003</t>
+  </si>
+  <si>
+    <t>2004/2005</t>
+  </si>
+  <si>
+    <t>2006/2007</t>
+  </si>
+  <si>
+    <t>2008/2009</t>
+  </si>
+  <si>
+    <t>2010/2011</t>
+  </si>
+  <si>
+    <t>2012/2013</t>
+  </si>
+  <si>
+    <t>2014/2015</t>
+  </si>
+  <si>
+    <t>2016/2017</t>
   </si>
 </sst>
 </file>
@@ -1722,7 +1753,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1820,22 +1851,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1843,6 +1862,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1853,6 +1875,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1883,6 +1917,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2184,10 +2222,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,9 +2239,10 @@
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2231,8 +2270,12 @@
       <c r="I1" s="28" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="62" t="s">
+        <v>270</v>
+      </c>
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2258,8 +2301,9 @@
       <c r="I2" s="34" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="36"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>184</v>
       </c>
@@ -2287,8 +2331,11 @@
       <c r="I3" s="35" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>185</v>
       </c>
@@ -2304,8 +2351,11 @@
       <c r="G4" s="11"/>
       <c r="H4" s="30"/>
       <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>186</v>
       </c>
@@ -2331,102 +2381,113 @@
         <v>16</v>
       </c>
       <c r="I5" s="26"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>187</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="G6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="42">
         <v>16</v>
       </c>
-      <c r="I6" s="36"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="37"/>
+      <c r="J6" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>188</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="36"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="36"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>189</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="42">
         <v>16</v>
       </c>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="37"/>
+      <c r="J8" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>190</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="36"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="36"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>191</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="48" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2435,163 +2496,182 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H10" s="44">
         <v>32</v>
       </c>
       <c r="I10" s="33" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="33" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>192</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="48"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="45"/>
       <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>193</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="36" t="s">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="45"/>
       <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>194</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="45"/>
       <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>195</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="45"/>
       <c r="I14" s="26"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>196</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="40" t="s">
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="43" t="s">
+      <c r="G15" s="49"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="39" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="35" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>211</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="44"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="36"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>212</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="45"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="36"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>198</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="42">
         <v>16</v>
       </c>
-      <c r="I18" s="36"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="37"/>
+      <c r="J18" s="36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>197</v>
       </c>
@@ -2603,13 +2683,15 @@
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
-      <c r="H19" s="46"/>
+      <c r="H19" s="43"/>
       <c r="I19" s="38"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>215</v>
       </c>
@@ -2623,18 +2705,15 @@
       <c r="G21" s="8"/>
       <c r="H21" s="31"/>
       <c r="I21" s="8"/>
+      <c r="J21" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -2651,11 +2730,15 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2799,10 +2882,10 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="37" t="s">
         <v>177</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -2822,8 +2905,8 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="9" t="s">
         <v>220</v>
       </c>
@@ -2841,10 +2924,10 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="37" t="s">
         <v>178</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2864,8 +2947,8 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="9" t="s">
         <v>220</v>
       </c>
@@ -2929,10 +3012,10 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="37" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -2952,8 +3035,8 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="9" t="s">
         <v>220</v>
       </c>
@@ -2971,8 +3054,8 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="9" t="s">
         <v>220</v>
       </c>
@@ -2990,10 +3073,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="48" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3013,8 +3096,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3032,8 +3115,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3051,10 +3134,10 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="37" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -3110,16 +3193,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3150,33 +3233,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="51" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -3211,18 +3294,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="55" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="56"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -19091,28 +19174,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
add mark for request to open ports for SHKUch-3,4,8
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -20,7 +20,7 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1574,7 +1574,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1753,7 +1753,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1845,16 +1845,32 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1862,9 +1878,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1875,18 +1888,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1919,9 +1920,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2225,7 +2228,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,10 +2273,10 @@
       <c r="I1" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="K1" s="61"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -2301,7 +2304,7 @@
       <c r="I2" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="J2" s="36"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -2328,7 +2331,7 @@
       <c r="H3" s="29">
         <v>16</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="33" t="s">
         <v>268</v>
       </c>
       <c r="J3" s="9" t="s">
@@ -2380,7 +2383,7 @@
       <c r="H5" s="29">
         <v>16</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="9" t="s">
         <v>272</v>
       </c>
@@ -2392,25 +2395,25 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="41">
         <v>16</v>
       </c>
-      <c r="I6" s="37"/>
+      <c r="I6" s="63"/>
       <c r="J6" s="9" t="s">
         <v>273</v>
       </c>
@@ -2422,14 +2425,14 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -2438,25 +2441,25 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="41">
         <v>16</v>
       </c>
-      <c r="I8" s="37"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="9" t="s">
         <v>274</v>
       </c>
@@ -2468,14 +2471,14 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -2484,10 +2487,10 @@
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="42" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2496,10 +2499,10 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="49">
         <v>32</v>
       </c>
       <c r="I10" s="33" t="s">
@@ -2516,17 +2519,17 @@
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="26"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="62"/>
       <c r="J11" s="9" t="s">
         <v>276</v>
       </c>
@@ -2538,16 +2541,16 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="37" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="49"/>
-      <c r="H12" s="45"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="26"/>
       <c r="J12" s="9" t="s">
         <v>277</v>
@@ -2560,14 +2563,14 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="45"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="26"/>
-      <c r="J13" s="36"/>
+      <c r="J13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2576,14 +2579,14 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="45"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="26"/>
-      <c r="J14" s="36"/>
+      <c r="J14" s="35"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -2592,17 +2595,17 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="48" t="s">
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="49"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="39" t="s">
+      <c r="G15" s="43"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="45" t="s">
         <v>265</v>
       </c>
       <c r="J15" s="33" t="s">
@@ -2616,14 +2619,14 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="36"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -2632,14 +2635,14 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="36"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -2648,26 +2651,26 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="41">
         <v>16</v>
       </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="36" t="s">
+      <c r="I18" s="38"/>
+      <c r="J18" s="35" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2678,18 +2681,18 @@
       <c r="B19" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="36"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I20" s="8"/>
-      <c r="J20" s="36"/>
+      <c r="J20" s="35"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -2705,15 +2708,19 @@
       <c r="G21" s="8"/>
       <c r="H21" s="31"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="36"/>
+      <c r="J21" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -2730,15 +2737,11 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2882,10 +2885,10 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>177</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -2905,8 +2908,8 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="9" t="s">
         <v>220</v>
       </c>
@@ -2924,10 +2927,10 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>178</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2947,8 +2950,8 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="9" t="s">
         <v>220</v>
       </c>
@@ -3012,10 +3015,10 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="38" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -3035,8 +3038,8 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="9" t="s">
         <v>220</v>
       </c>
@@ -3054,8 +3057,8 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="9" t="s">
         <v>220</v>
       </c>
@@ -3073,10 +3076,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="42" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3096,8 +3099,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3115,8 +3118,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3134,10 +3137,10 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="38" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -3157,8 +3160,8 @@
       <c r="B19" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="9" t="s">
         <v>220</v>
       </c>
@@ -3193,16 +3196,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3233,33 +3236,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="52" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="53" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="55"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -3294,18 +3297,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -19174,28 +19177,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="59" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
add information about request to open ports for SHKUch-3,4,8
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="281">
   <si>
     <t>Устройство</t>
   </si>
@@ -1444,6 +1444,13 @@
   </si>
   <si>
     <t>2016/2017</t>
+  </si>
+  <si>
+    <t>порт Fa0/24</t>
+  </si>
+  <si>
+    <t>1 - порт G0/2/1
+2 - подключить к неиспользуемому порту и сообщить MAC-адрес.</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1852,6 +1859,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1869,6 +1879,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1921,10 +1934,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2228,7 +2238,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2393,9 @@
       <c r="H5" s="29">
         <v>16</v>
       </c>
-      <c r="I5" s="62"/>
+      <c r="I5" s="38" t="s">
+        <v>279</v>
+      </c>
       <c r="J5" s="9" t="s">
         <v>272</v>
       </c>
@@ -2395,25 +2407,27 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="42">
         <v>16</v>
       </c>
-      <c r="I6" s="63"/>
+      <c r="I6" s="64" t="s">
+        <v>280</v>
+      </c>
       <c r="J6" s="9" t="s">
         <v>273</v>
       </c>
@@ -2425,13 +2439,13 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="63"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2441,25 +2455,25 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="42">
         <v>16</v>
       </c>
-      <c r="I8" s="38"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="9" t="s">
         <v>274</v>
       </c>
@@ -2471,13 +2485,13 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2487,10 +2501,10 @@
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="43" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2499,10 +2513,10 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="51">
         <v>32</v>
       </c>
       <c r="I10" s="33" t="s">
@@ -2519,17 +2533,19 @@
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="62"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="38" t="s">
+        <v>279</v>
+      </c>
       <c r="J11" s="9" t="s">
         <v>276</v>
       </c>
@@ -2541,16 +2557,16 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="38" t="s">
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="50"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="52"/>
       <c r="I12" s="26"/>
       <c r="J12" s="9" t="s">
         <v>277</v>
@@ -2563,12 +2579,12 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="52"/>
       <c r="I13" s="26"/>
       <c r="J13" s="35"/>
     </row>
@@ -2579,12 +2595,12 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="50"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="52"/>
       <c r="I14" s="26"/>
       <c r="J14" s="35"/>
     </row>
@@ -2595,17 +2611,17 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="42" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="45" t="s">
+      <c r="G15" s="44"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="47" t="s">
         <v>265</v>
       </c>
       <c r="J15" s="33" t="s">
@@ -2619,13 +2635,13 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="48"/>
       <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2635,13 +2651,13 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2651,25 +2667,25 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H18" s="42">
         <v>16</v>
       </c>
-      <c r="I18" s="38"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="35" t="s">
         <v>278</v>
       </c>
@@ -2681,13 +2697,13 @@
       <c r="B19" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2885,10 +2901,10 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="39" t="s">
         <v>177</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -2908,8 +2924,8 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="9" t="s">
         <v>220</v>
       </c>
@@ -2927,10 +2943,10 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="39" t="s">
         <v>178</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2950,8 +2966,8 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="9" t="s">
         <v>220</v>
       </c>
@@ -3015,10 +3031,10 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="39" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -3038,8 +3054,8 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="9" t="s">
         <v>220</v>
       </c>
@@ -3057,8 +3073,8 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="9" t="s">
         <v>220</v>
       </c>
@@ -3076,10 +3092,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3099,8 +3115,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3118,8 +3134,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3137,10 +3153,10 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="39" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -3160,8 +3176,8 @@
       <c r="B19" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="9" t="s">
         <v>220</v>
       </c>
@@ -3236,33 +3252,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="53" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="55" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="55"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -3297,18 +3313,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -19177,28 +19193,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="61" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
fix IDB port for ShKUch-11
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="282">
   <si>
     <t>Устройство</t>
   </si>
@@ -1451,6 +1451,9 @@
   <si>
     <t>1 - порт G0/2/1
 2 - подключить к неиспользуемому порту и сообщить MAC-адрес.</t>
+  </si>
+  <si>
+    <t>2018/2019</t>
   </si>
 </sst>
 </file>
@@ -1865,25 +1868,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1891,6 +1882,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1901,6 +1895,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1931,9 +1937,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2238,7 +2241,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,7 +2413,7 @@
       <c r="C6" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="51" t="s">
         <v>36</v>
       </c>
       <c r="E6" s="39" t="s">
@@ -2422,10 +2425,10 @@
       <c r="G6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="46">
         <v>16</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="40" t="s">
         <v>280</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -2444,8 +2447,8 @@
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2458,7 +2461,7 @@
       <c r="C8" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="51" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="39" t="s">
@@ -2470,7 +2473,7 @@
       <c r="G8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="46">
         <v>16</v>
       </c>
       <c r="I8" s="39"/>
@@ -2490,7 +2493,7 @@
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
-      <c r="H9" s="42"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="39"/>
       <c r="J9" s="35"/>
     </row>
@@ -2501,10 +2504,10 @@
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="52" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2513,10 +2516,10 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="48">
         <v>32</v>
       </c>
       <c r="I10" s="33" t="s">
@@ -2533,16 +2536,16 @@
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="44"/>
-      <c r="H11" s="52"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="49"/>
       <c r="I11" s="38" t="s">
         <v>279</v>
       </c>
@@ -2557,16 +2560,16 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="39" t="s">
         <v>166</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="52"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="26"/>
       <c r="J12" s="9" t="s">
         <v>277</v>
@@ -2579,12 +2582,12 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="52"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="49"/>
       <c r="I13" s="26"/>
       <c r="J13" s="35"/>
     </row>
@@ -2595,12 +2598,12 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="52"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="26"/>
       <c r="J14" s="35"/>
     </row>
@@ -2611,17 +2614,17 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="43" t="s">
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="47" t="s">
+      <c r="G15" s="53"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="43" t="s">
         <v>265</v>
       </c>
       <c r="J15" s="33" t="s">
@@ -2635,13 +2638,13 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="48"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="44"/>
       <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2651,13 +2654,13 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2670,7 +2673,7 @@
       <c r="C18" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="51" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="39" t="s">
@@ -2682,12 +2685,12 @@
       <c r="G18" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="46">
         <v>16</v>
       </c>
       <c r="I18" s="39"/>
       <c r="J18" s="35" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2697,13 +2700,13 @@
       <c r="B19" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="42"/>
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2728,15 +2731,11 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -2753,11 +2752,15 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -3092,10 +3095,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="52" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3115,8 +3118,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3134,8 +3137,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3176,8 +3179,8 @@
       <c r="B19" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="9" t="s">
         <v>220</v>
       </c>
@@ -3212,16 +3215,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3252,33 +3255,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="55" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="56" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -3313,18 +3316,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -19193,28 +19196,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="62" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
add SHKUch-1 to IDB
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr updateLinks="never" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\prj_ASU\AMKP\git\gasCollectionPrj\Documentation\"/>
@@ -2241,7 +2241,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2347,7 @@
       <c r="I3" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="33" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add info about SHKUch-4 to Excel
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -1868,13 +1868,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1882,9 +1897,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1895,18 +1907,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -2241,7 +2241,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2413,7 @@
       <c r="C6" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="40" t="s">
         <v>36</v>
       </c>
       <c r="E6" s="39" t="s">
@@ -2425,13 +2425,13 @@
       <c r="G6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="42">
         <v>16</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="46" t="s">
         <v>280</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="33" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2447,8 +2447,8 @@
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="41"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
       <c r="C8" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="40" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="39" t="s">
@@ -2473,7 +2473,7 @@
       <c r="G8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="42">
         <v>16</v>
       </c>
       <c r="I8" s="39"/>
@@ -2493,7 +2493,7 @@
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
-      <c r="H9" s="46"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="39"/>
       <c r="J9" s="35"/>
     </row>
@@ -2504,10 +2504,10 @@
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="43" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2516,10 +2516,10 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="52">
         <v>32</v>
       </c>
       <c r="I10" s="33" t="s">
@@ -2536,16 +2536,16 @@
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="49"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="53"/>
       <c r="I11" s="38" t="s">
         <v>279</v>
       </c>
@@ -2560,16 +2560,16 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="39" t="s">
         <v>166</v>
       </c>
       <c r="F12" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="49"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="26"/>
       <c r="J12" s="9" t="s">
         <v>277</v>
@@ -2582,12 +2582,12 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="49"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="53"/>
       <c r="I13" s="26"/>
       <c r="J13" s="35"/>
     </row>
@@ -2598,12 +2598,12 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="49"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="53"/>
       <c r="I14" s="26"/>
       <c r="J14" s="35"/>
     </row>
@@ -2614,17 +2614,17 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="52" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="43" t="s">
+      <c r="G15" s="44"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="48" t="s">
         <v>265</v>
       </c>
       <c r="J15" s="33" t="s">
@@ -2638,13 +2638,13 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2654,13 +2654,13 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
       <c r="C18" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="40" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="39" t="s">
@@ -2685,7 +2685,7 @@
       <c r="G18" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="42">
         <v>16</v>
       </c>
       <c r="I18" s="39"/>
@@ -2700,13 +2700,13 @@
       <c r="B19" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="41"/>
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2731,11 +2731,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -2752,15 +2756,11 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -3095,10 +3095,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3118,8 +3118,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3137,8 +3137,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3179,8 +3179,8 @@
       <c r="B19" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="9" t="s">
         <v>220</v>
       </c>
@@ -3215,16 +3215,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add ip an port for SHKUch-2,3
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="never" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\prj_ASU\AMKP\git\gasCollectionPrj\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\prj_ASU\AMKP\.git\gasCollectionPrj\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="286">
   <si>
     <t>Устройство</t>
   </si>
@@ -1454,6 +1454,18 @@
   </si>
   <si>
     <t>2018/2019</t>
+  </si>
+  <si>
+    <t>порт 7, 8</t>
+  </si>
+  <si>
+    <t>10.27.142.194</t>
+  </si>
+  <si>
+    <t>10.27.142.193</t>
+  </si>
+  <si>
+    <t>010.027.142.192/28</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1830,9 +1842,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1840,9 +1849,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1868,13 +1874,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1882,9 +1906,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1895,18 +1916,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1938,6 +1947,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2241,7 +2256,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,16 +2295,16 @@
       <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="K1" s="36"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -2311,13 +2326,13 @@
       <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="28">
         <v>8</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -2341,13 +2356,13 @@
       <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>16</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="31" t="s">
         <v>269</v>
       </c>
     </row>
@@ -2355,18 +2370,30 @@
       <c r="A4" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>36</v>
+      </c>
       <c r="E4" s="5" t="s">
         <v>160</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="11"/>
+      <c r="G4" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="H4" s="38">
+        <v>16</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>282</v>
+      </c>
       <c r="J4" s="9" t="s">
         <v>271</v>
       </c>
@@ -2393,10 +2420,10 @@
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="28">
         <v>16</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="31" t="s">
         <v>279</v>
       </c>
       <c r="J5" s="9" t="s">
@@ -2410,28 +2437,28 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="43">
         <v>16</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="64" t="s">
         <v>280</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="31" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2442,14 +2469,14 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="35"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -2458,25 +2485,25 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="43">
         <v>16</v>
       </c>
-      <c r="I8" s="41"/>
+      <c r="I8" s="65"/>
       <c r="J8" s="9" t="s">
         <v>274</v>
       </c>
@@ -2488,14 +2515,14 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="35"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -2504,10 +2531,10 @@
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="44" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2516,16 +2543,16 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="51">
         <v>32</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="31" t="s">
         <v>275</v>
       </c>
     </row>
@@ -2536,17 +2563,17 @@
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="38" t="s">
+      <c r="G11" s="45"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="36" t="s">
         <v>279</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -2560,17 +2587,17 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="39" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="26"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="9" t="s">
         <v>277</v>
       </c>
@@ -2582,14 +2609,14 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="35"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="44"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2598,14 +2625,14 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="35"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -2614,20 +2641,20 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="52" t="s">
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="53"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="43" t="s">
+      <c r="G15" s="45"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="31" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2638,14 +2665,14 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="35"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -2654,14 +2681,14 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="35"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -2670,26 +2697,26 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="43">
         <v>16</v>
       </c>
-      <c r="I18" s="39"/>
-      <c r="J18" s="35" t="s">
+      <c r="I18" s="40"/>
+      <c r="J18" s="37" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2705,13 +2732,13 @@
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
-      <c r="H19" s="47"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="42"/>
-      <c r="J19" s="35"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I20" s="8"/>
-      <c r="J20" s="35"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -2725,17 +2752,24 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="31"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="35"/>
+      <c r="J21" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+  <mergeCells count="33">
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I12:I14"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -2752,15 +2786,11 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2904,10 +2934,10 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="40" t="s">
         <v>177</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -2927,8 +2957,8 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="9" t="s">
         <v>220</v>
       </c>
@@ -2946,10 +2976,10 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="40" t="s">
         <v>178</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2969,8 +2999,8 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="9" t="s">
         <v>220</v>
       </c>
@@ -3034,10 +3064,10 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="40" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -3057,8 +3087,8 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="9" t="s">
         <v>220</v>
       </c>
@@ -3076,8 +3106,8 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="9" t="s">
         <v>220</v>
       </c>
@@ -3095,10 +3125,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="44" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3118,8 +3148,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3137,8 +3167,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3156,10 +3186,10 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="40" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -3215,16 +3245,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3255,33 +3285,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="56" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="55" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -3316,18 +3346,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -3353,7 +3383,7 @@
       <c r="I6" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3381,7 +3411,7 @@
       <c r="I7" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3409,7 +3439,7 @@
       <c r="I8" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3437,7 +3467,7 @@
       <c r="I9" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3465,7 +3495,7 @@
       <c r="I10" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3493,7 +3523,7 @@
       <c r="I11" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3521,7 +3551,7 @@
       <c r="I12" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3549,7 +3579,7 @@
       <c r="I13" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3577,7 +3607,7 @@
       <c r="I14" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3605,7 +3635,7 @@
       <c r="I15" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="26" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3633,7 +3663,7 @@
       <c r="I16" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="26" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3661,7 +3691,7 @@
       <c r="I17" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="26" t="s">
         <v>261</v>
       </c>
     </row>
@@ -19196,28 +19226,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="61" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -19304,7 +19334,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -19321,7 +19351,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -19338,7 +19368,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Add ip an port for SHKUch-5 AND request about SHKUch-9, 11
</commit_message>
<xml_diff>
--- a/Documentation/IP_Adress_AMKP.xlsx
+++ b/Documentation/IP_Adress_AMKP.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="288">
   <si>
     <t>Устройство</t>
   </si>
@@ -1467,12 +1467,19 @@
   <si>
     <t>010.027.142.192/28</t>
   </si>
+  <si>
+    <t>запрос от 16.01.2017</t>
+  </si>
+  <si>
+    <t>Fa 0/3
+Fa 0/5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1550,8 +1557,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1598,6 +1612,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1771,11 +1790,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1880,25 +1900,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1906,6 +1923,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1916,6 +1936,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1948,14 +1974,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Нейтральный" xfId="2" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
@@ -2256,7 +2290,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I8" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,25 +2471,25 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="49">
         <v>16</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="43" t="s">
         <v>280</v>
       </c>
       <c r="J6" s="31" t="s">
@@ -2469,13 +2503,13 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="65"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2485,25 +2519,27 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="49">
         <v>16</v>
       </c>
-      <c r="I8" s="65"/>
+      <c r="I8" s="43" t="s">
+        <v>287</v>
+      </c>
       <c r="J8" s="9" t="s">
         <v>274</v>
       </c>
@@ -2515,13 +2551,13 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="65"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2531,10 +2567,10 @@
       <c r="B10" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="40" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2543,7 +2579,7 @@
       <c r="F10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="40" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="51">
@@ -2563,15 +2599,15 @@
       <c r="B11" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G11" s="45"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="52"/>
       <c r="I11" s="36" t="s">
         <v>279</v>
@@ -2587,17 +2623,19 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="40" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="52"/>
-      <c r="I12" s="44"/>
+      <c r="I12" s="66" t="s">
+        <v>286</v>
+      </c>
       <c r="J12" s="9" t="s">
         <v>277</v>
       </c>
@@ -2609,14 +2647,14 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="45"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="52"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="44"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2625,14 +2663,14 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="45"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="52"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="41"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -2641,17 +2679,17 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="44" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="45"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="52"/>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="46" t="s">
         <v>265</v>
       </c>
       <c r="J15" s="31" t="s">
@@ -2665,14 +2703,14 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="52"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="44"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -2681,14 +2719,14 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="53"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="46"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -2697,25 +2735,27 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="43">
+      <c r="H18" s="49">
         <v>16</v>
       </c>
-      <c r="I18" s="40"/>
+      <c r="I18" s="69" t="s">
+        <v>286</v>
+      </c>
       <c r="J18" s="37" t="s">
         <v>281</v>
       </c>
@@ -2727,13 +2767,13 @@
       <c r="B19" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="50"/>
-      <c r="I19" s="42"/>
+      <c r="I19" s="70"/>
       <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2758,18 +2798,11 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -2786,11 +2819,18 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="E12:E14"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="40" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2934,10 +2974,10 @@
       <c r="B6" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="42" t="s">
         <v>177</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -2957,8 +2997,8 @@
       <c r="B7" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="9" t="s">
         <v>220</v>
       </c>
@@ -2976,10 +3016,10 @@
       <c r="B8" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="42" t="s">
         <v>178</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2999,8 +3039,8 @@
       <c r="B9" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="9" t="s">
         <v>220</v>
       </c>
@@ -3064,10 +3104,10 @@
       <c r="B12" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="42" t="s">
         <v>181</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -3087,8 +3127,8 @@
       <c r="B13" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="9" t="s">
         <v>220</v>
       </c>
@@ -3106,8 +3146,8 @@
       <c r="B14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="9" t="s">
         <v>220</v>
       </c>
@@ -3125,10 +3165,10 @@
       <c r="B15" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="40" t="s">
         <v>182</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -3148,8 +3188,8 @@
       <c r="B16" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="9" t="s">
         <v>220</v>
       </c>
@@ -3167,8 +3207,8 @@
       <c r="B17" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="9" t="s">
         <v>220</v>
       </c>
@@ -3186,10 +3226,10 @@
       <c r="B18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="42" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -3209,8 +3249,8 @@
       <c r="B19" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="9" t="s">
         <v>220</v>
       </c>
@@ -3245,16 +3285,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3285,33 +3325,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="56" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="57" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="55" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="57" t="s">
         <v>227</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="57"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="59"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -3346,18 +3386,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -19226,28 +19266,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">

</xml_diff>